<commit_message>
Update IRAP procedural parameters, stimuli, and publication status.xlsx
added note that sexuality studies examine men only
</commit_message>
<xml_diff>
--- a/measures/IRAP procedural parameters, stimuli, and publication status.xlsx
+++ b/measures/IRAP procedural parameters, stimuli, and publication status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/irap-reliability-meta-analysis/measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5209CAD3-5552-1448-A692-785752C8FD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA977C2-154A-3647-9075-96F210911559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="28120" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="740" windowWidth="28120" windowHeight="18380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="340">
   <si>
     <t>Religion</t>
   </si>
@@ -415,9 +415,6 @@
   </si>
   <si>
     <t>[disgusting images: rotten meat, a large maggot, bloody hand, diseased mouth cavity, toilet with feces, burned face]</t>
-  </si>
-  <si>
-    <t>Images taken from the International Affective Picture System and found online, see Hughes, Hussey, Corrigan, Jolie, Murphy &amp; Barnes-Holmes (2016)</t>
   </si>
   <si>
     <t xml:space="preserve">During the next part of the experiment PLEASE RESPOND AS IF GOOD WORDS ARE GOOD AND BAD WORDS ARE BAD. </t>
@@ -1396,9 +1393,6 @@
     <t>Convenience sample of undergraduate students at a Belgian university. Participants were paid either €5or course credit.</t>
   </si>
   <si>
-    <t>Note that stimuli were presented in Dutch. English translations are presented here.</t>
-  </si>
-  <si>
     <t>English translation:
 bad
 unpleasant
@@ -1520,6 +1514,27 @@
   </si>
   <si>
     <t>Gender stereotypes (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convenience sample of undergraduate students at an Irish university who identified as both male and either gay or straight. No compensation was offered. </t>
+  </si>
+  <si>
+    <t>Hughes, Hussey, Corrigan, Jolie, Murphy, &amp; Barnes-Holmes. (2016) Faking revisited: Exerting strategic control over performance on the Implicit Relational Assessment Procedure: IRAP faking.</t>
+  </si>
+  <si>
+    <t>See "image stimuli" folder for images.  Note that only the baseline IRAP are included (i.e., prior to faking instructions).</t>
+  </si>
+  <si>
+    <t>Images taken from the International Affective Picture System (IAPS: Lang, Bradley, &amp; Cuthbert, 1997), which is proprietary and thereore cannot be distriuted here. Male picture numbers: 4460, 4500, 4534, 4550, 4561; female picture numbers: 4141, 4142, 4210, 4240, 4235.
+Note that only the baseline IRAP are included (i.e., prior to faking instructions).</t>
+  </si>
+  <si>
+    <t>Note that stimuli were presented in Dutch. English translations are presented here.
+Note that only the baseline IRAP are included (i.e., prior to faking instructions).</t>
+  </si>
+  <si>
+    <t>Images taken from the International Affective Picture System and found online, see Hughes, Hussey, Corrigan, Jolie, Murphy &amp; Barnes-Holmes (2016). 
+Note that only the baseline IRAP are included (i.e., prior to faking instructions).</t>
   </si>
 </sst>
 </file>
@@ -2308,9 +2323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2340,10 +2355,10 @@
   <sheetData>
     <row r="1" spans="1:23" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>18</v>
@@ -2352,16 +2367,16 @@
         <v>19</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>329</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>331</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>55</v>
@@ -2373,13 +2388,13 @@
         <v>21</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="N1" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>20</v>
@@ -2391,19 +2406,19 @@
         <v>35</v>
       </c>
       <c r="R1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>39</v>
@@ -2414,7 +2429,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2429,16 +2444,16 @@
         <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="I2" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>15</v>
@@ -2450,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O2" s="16" t="s">
         <v>16</v>
@@ -2462,22 +2477,22 @@
         <v>2000</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S2" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="T2" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="U2" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -2485,7 +2500,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
@@ -2500,16 +2515,16 @@
         <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="I3" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>15</v>
@@ -2521,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>17</v>
@@ -2533,22 +2548,22 @@
         <v>2000</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S3" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="T3" s="8">
         <v>2016</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -2556,7 +2571,7 @@
         <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>63</v>
@@ -2565,22 +2580,22 @@
         <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="I4" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>59</v>
@@ -2592,7 +2607,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O4" s="15" t="s">
         <v>17</v>
@@ -2604,22 +2619,22 @@
         <v>2000</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -2627,7 +2642,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>64</v>
@@ -2636,22 +2651,22 @@
         <v>65</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="G5" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="I5" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>59</v>
@@ -2663,7 +2678,7 @@
         <v>3</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O5" s="15" t="s">
         <v>17</v>
@@ -2675,22 +2690,22 @@
         <v>2000</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -2698,7 +2713,7 @@
         <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>57</v>
@@ -2707,22 +2722,22 @@
         <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="I6" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J6" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>59</v>
@@ -2734,7 +2749,7 @@
         <v>3</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O6" s="15" t="s">
         <v>17</v>
@@ -2746,22 +2761,22 @@
         <v>2000</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="119" x14ac:dyDescent="0.2">
@@ -2769,7 +2784,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>60</v>
@@ -2778,22 +2793,22 @@
         <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G7" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="I7" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J7" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K7" s="15" t="s">
         <v>59</v>
@@ -2805,7 +2820,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O7" s="15" t="s">
         <v>17</v>
@@ -2817,22 +2832,22 @@
         <v>2000</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -2840,7 +2855,7 @@
         <v>104</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
@@ -2849,22 +2864,22 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="I8" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>59</v>
@@ -2876,7 +2891,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O8" s="16" t="s">
         <v>17</v>
@@ -2888,22 +2903,22 @@
         <v>2000</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T8" s="8">
         <v>2013</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -2911,7 +2926,7 @@
         <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>11</v>
@@ -2926,16 +2941,16 @@
         <v>31</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I9" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K9" s="15" t="s">
         <v>59</v>
@@ -2947,7 +2962,7 @@
         <v>3</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>17</v>
@@ -2959,22 +2974,22 @@
         <v>2000</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T9" s="8">
         <v>2013</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -2982,7 +2997,7 @@
         <v>106</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -2997,16 +3012,16 @@
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="I10" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>59</v>
@@ -3018,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O10" s="16" t="s">
         <v>17</v>
@@ -3030,54 +3045,54 @@
         <v>2000</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T10" s="8">
         <v>2013</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="I11" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>184</v>
-      </c>
-      <c r="J11" s="18" t="s">
-        <v>185</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>59</v>
@@ -3089,7 +3104,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O11" s="16" t="s">
         <v>17</v>
@@ -3101,54 +3116,54 @@
         <v>2000</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T11" s="8">
         <v>2013</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W11" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="187" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="E12" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="G12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="I12" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>59</v>
@@ -3160,7 +3175,7 @@
         <v>3</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O12" s="16" t="s">
         <v>17</v>
@@ -3169,33 +3184,33 @@
         <v>80</v>
       </c>
       <c r="Q12" s="17">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T12" s="8">
         <v>2014</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="272" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>70</v>
@@ -3204,10 +3219,10 @@
         <v>71</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>129</v>
@@ -3216,10 +3231,10 @@
         <v>128</v>
       </c>
       <c r="I13" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K13" s="15" t="s">
         <v>59</v>
@@ -3231,7 +3246,7 @@
         <v>3</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O13" s="16" t="s">
         <v>17</v>
@@ -3243,22 +3258,22 @@
         <v>2000</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S13" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="T13" s="8">
         <v>2013</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>130</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -3266,7 +3281,7 @@
         <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -3275,22 +3290,22 @@
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="G14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="I14" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>15</v>
@@ -3302,7 +3317,7 @@
         <v>3</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O14" s="16" t="s">
         <v>16</v>
@@ -3314,30 +3329,30 @@
         <v>2000</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S14" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T14" s="8">
         <v>2013</v>
       </c>
       <c r="U14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="V14" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="V14" s="14" t="s">
-        <v>173</v>
-      </c>
       <c r="W14" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>72</v>
@@ -3346,22 +3361,22 @@
         <v>73</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="I15" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>15</v>
@@ -3373,7 +3388,7 @@
         <v>3</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O15" s="16" t="s">
         <v>16</v>
@@ -3385,30 +3400,30 @@
         <v>2000</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S15" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="T15" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="T15" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="U15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="V15" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="V15" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="W15" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>51</v>
@@ -3423,16 +3438,16 @@
         <v>44</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="I16" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J16" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>15</v>
@@ -3444,7 +3459,7 @@
         <v>3</v>
       </c>
       <c r="N16" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O16" s="16" t="s">
         <v>16</v>
@@ -3456,54 +3471,54 @@
         <v>2000</v>
       </c>
       <c r="R16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S16" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="S16" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="T16" s="8">
         <v>2016</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="136" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>280</v>
-      </c>
       <c r="I17" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J17" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>59</v>
@@ -3515,7 +3530,7 @@
         <v>3</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O17" s="21" t="s">
         <v>17</v>
@@ -3527,54 +3542,54 @@
         <v>2000</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W17" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="153" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="I18" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>59</v>
@@ -3586,7 +3601,7 @@
         <v>3</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O18" s="16" t="s">
         <v>17</v>
@@ -3598,22 +3613,22 @@
         <v>2000</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T18" s="8">
         <v>2015</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -3621,7 +3636,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
@@ -3636,16 +3651,16 @@
         <v>28</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="I19" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J19" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J19" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>15</v>
@@ -3657,7 +3672,7 @@
         <v>3</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O19" s="16" t="s">
         <v>16</v>
@@ -3669,19 +3684,19 @@
         <v>2000</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S19" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T19" s="8">
         <v>2013</v>
       </c>
       <c r="U19" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>40</v>
@@ -3689,34 +3704,34 @@
     </row>
     <row r="20" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="G20" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="I20" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J20" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>59</v>
@@ -3728,7 +3743,7 @@
         <v>3</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O20" s="16" t="s">
         <v>17</v>
@@ -3740,22 +3755,22 @@
         <v>2000</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T20" s="8">
         <v>2014</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -3763,7 +3778,7 @@
         <v>107</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>78</v>
@@ -3778,16 +3793,16 @@
         <v>81</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="I21" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J21" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J21" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>15</v>
@@ -3799,7 +3814,7 @@
         <v>3</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O21" s="15" t="s">
         <v>16</v>
@@ -3811,22 +3826,22 @@
         <v>2500</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S21" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T21" s="8">
         <v>2014</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W21" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -3834,7 +3849,7 @@
         <v>108</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>84</v>
@@ -3849,16 +3864,16 @@
         <v>83</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="I22" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>15</v>
@@ -3870,7 +3885,7 @@
         <v>3</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O22" s="15" t="s">
         <v>16</v>
@@ -3882,22 +3897,22 @@
         <v>2500</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S22" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T22" s="8">
         <v>2014</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W22" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -3905,7 +3920,7 @@
         <v>109</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>86</v>
@@ -3920,16 +3935,16 @@
         <v>89</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="I23" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J23" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>15</v>
@@ -3941,7 +3956,7 @@
         <v>3</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O23" s="15" t="s">
         <v>16</v>
@@ -3953,22 +3968,22 @@
         <v>2500</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S23" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T23" s="8">
         <v>2014</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W23" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -3976,7 +3991,7 @@
         <v>110</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>96</v>
@@ -3991,16 +4006,16 @@
         <v>91</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="I24" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J24" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J24" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>15</v>
@@ -4012,7 +4027,7 @@
         <v>3</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O24" s="15" t="s">
         <v>16</v>
@@ -4024,22 +4039,22 @@
         <v>2500</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S24" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T24" s="8">
         <v>2014</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W24" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4047,7 +4062,7 @@
         <v>111</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>94</v>
@@ -4062,16 +4077,16 @@
         <v>93</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="I25" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J25" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>15</v>
@@ -4083,7 +4098,7 @@
         <v>3</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O25" s="15" t="s">
         <v>16</v>
@@ -4095,22 +4110,22 @@
         <v>2500</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S25" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T25" s="8">
         <v>2014</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4118,7 +4133,7 @@
         <v>112</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
@@ -4133,16 +4148,16 @@
         <v>26</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="I26" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>144</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>15</v>
@@ -4154,7 +4169,7 @@
         <v>3</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O26" s="16" t="s">
         <v>16</v>
@@ -4166,22 +4181,22 @@
         <v>2000</v>
       </c>
       <c r="R26" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S26" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="S26" s="12" t="s">
+      <c r="T26" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="T26" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="U26" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="238" x14ac:dyDescent="0.2">
@@ -4189,7 +4204,7 @@
         <v>113</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
@@ -4204,16 +4219,16 @@
         <v>37</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="I27" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J27" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>59</v>
@@ -4225,7 +4240,7 @@
         <v>3</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O27" s="16" t="s">
         <v>17</v>
@@ -4237,22 +4252,22 @@
         <v>2000</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S27" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T27" s="8">
         <v>2013</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>286</v>
+        <v>335</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>40</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4260,7 +4275,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>1</v>
@@ -4275,16 +4290,16 @@
         <v>24</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="I28" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J28" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K28" s="16" t="s">
         <v>15</v>
@@ -4296,7 +4311,7 @@
         <v>3</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O28" s="16" t="s">
         <v>16</v>
@@ -4308,22 +4323,22 @@
         <v>2000</v>
       </c>
       <c r="R28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S28" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="S28" s="12" t="s">
+      <c r="T28" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="T28" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="U28" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4331,7 +4346,7 @@
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>53</v>
@@ -4346,16 +4361,16 @@
         <v>46</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="I29" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J29" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K29" s="16" t="s">
         <v>15</v>
@@ -4367,7 +4382,7 @@
         <v>3</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O29" s="16" t="s">
         <v>17</v>
@@ -4379,30 +4394,30 @@
         <v>2000</v>
       </c>
       <c r="R29" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S29" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="S29" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="T29" s="8">
         <v>2016</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W29" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>66</v>
@@ -4417,16 +4432,16 @@
         <v>69</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="I30" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J30" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J30" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K30" s="16" t="s">
         <v>15</v>
@@ -4438,7 +4453,7 @@
         <v>3</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O30" s="16" t="s">
         <v>17</v>
@@ -4450,30 +4465,30 @@
         <v>2000</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S30" s="11" t="s">
-        <v>168</v>
+        <v>334</v>
       </c>
       <c r="T30" s="8">
         <v>2013</v>
       </c>
       <c r="U30" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="V30" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="V30" s="11" t="s">
-        <v>287</v>
-      </c>
       <c r="W30" s="1" t="s">
-        <v>125</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="170" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>66</v>
@@ -4488,16 +4503,16 @@
         <v>69</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="I31" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J31" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K31" s="16" t="s">
         <v>15</v>
@@ -4509,7 +4524,7 @@
         <v>3</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O31" s="16" t="s">
         <v>17</v>
@@ -4521,19 +4536,19 @@
         <v>2000</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S31" s="11" t="s">
-        <v>168</v>
+        <v>334</v>
       </c>
       <c r="T31" s="8">
         <v>2012</v>
       </c>
       <c r="U31" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V31" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>125</v>
@@ -4544,31 +4559,31 @@
         <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="E32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I32" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I32" s="23" t="s">
+      <c r="J32" s="23" t="s">
         <v>143</v>
-      </c>
-      <c r="J32" s="23" t="s">
-        <v>144</v>
       </c>
       <c r="K32" s="16" t="s">
         <v>15</v>
@@ -4580,7 +4595,7 @@
         <v>3</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O32" s="16" t="s">
         <v>16</v>
@@ -4592,54 +4607,54 @@
         <v>2000</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S32" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T32" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V32" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W32" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="E33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I33" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I33" s="23" t="s">
+      <c r="J33" s="23" t="s">
         <v>143</v>
-      </c>
-      <c r="J33" s="23" t="s">
-        <v>144</v>
       </c>
       <c r="K33" s="16" t="s">
         <v>15</v>
@@ -4651,7 +4666,7 @@
         <v>3</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O33" s="16" t="s">
         <v>16</v>
@@ -4663,22 +4678,22 @@
         <v>2000</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S33" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T33" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V33" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W33" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4686,31 +4701,31 @@
         <v>115</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="E34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="G34" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="I34" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J34" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J34" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K34" s="16" t="s">
         <v>15</v>
@@ -4722,7 +4737,7 @@
         <v>3</v>
       </c>
       <c r="N34" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O34" s="16" t="s">
         <v>16</v>
@@ -4734,22 +4749,22 @@
         <v>2000</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S34" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T34" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W34" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4757,31 +4772,31 @@
         <v>116</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="E35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="G35" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="I35" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J35" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J35" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K35" s="16" t="s">
         <v>15</v>
@@ -4793,7 +4808,7 @@
         <v>3</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O35" s="16" t="s">
         <v>16</v>
@@ -4805,22 +4820,22 @@
         <v>2000</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S35" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T35" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V35" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W35" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4828,31 +4843,31 @@
         <v>117</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="E36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="G36" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="I36" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J36" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K36" s="16" t="s">
         <v>15</v>
@@ -4864,7 +4879,7 @@
         <v>3</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O36" s="15" t="s">
         <v>16</v>
@@ -4876,22 +4891,22 @@
         <v>2000</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S36" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T36" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V36" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W36" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4899,31 +4914,31 @@
         <v>118</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="E37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="G37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="I37" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J37" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J37" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K37" s="16" t="s">
         <v>15</v>
@@ -4935,7 +4950,7 @@
         <v>3</v>
       </c>
       <c r="N37" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O37" s="15" t="s">
         <v>16</v>
@@ -4947,22 +4962,22 @@
         <v>2000</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S37" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T37" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V37" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W37" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -4970,31 +4985,31 @@
         <v>119</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="E38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="G38" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="I38" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J38" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J38" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K38" s="16" t="s">
         <v>15</v>
@@ -5006,7 +5021,7 @@
         <v>3</v>
       </c>
       <c r="N38" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O38" s="15" t="s">
         <v>16</v>
@@ -5018,22 +5033,22 @@
         <v>2000</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S38" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T38" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V38" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W38" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:23" s="11" customFormat="1" ht="136" x14ac:dyDescent="0.2">
@@ -5041,7 +5056,7 @@
         <v>121</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>74</v>
@@ -5056,16 +5071,16 @@
         <v>77</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="I39" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J39" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J39" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K39" s="16" t="s">
         <v>15</v>
@@ -5077,7 +5092,7 @@
         <v>3</v>
       </c>
       <c r="N39" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O39" s="16" t="s">
         <v>17</v>
@@ -5089,19 +5104,19 @@
         <v>2000</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S39" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T39" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="U39" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V39" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>124</v>
@@ -5112,7 +5127,7 @@
         <v>122</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>74</v>
@@ -5127,16 +5142,16 @@
         <v>77</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I40" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J40" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J40" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K40" s="16" t="s">
         <v>15</v>
@@ -5148,7 +5163,7 @@
         <v>3</v>
       </c>
       <c r="N40" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O40" s="16" t="s">
         <v>17</v>
@@ -5160,19 +5175,19 @@
         <v>2000</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S40" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T40" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="U40" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V40" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W40" s="1" t="s">
         <v>124</v>
@@ -5183,7 +5198,7 @@
         <v>123</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>74</v>
@@ -5198,16 +5213,16 @@
         <v>77</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I41" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J41" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="K41" s="16" t="s">
         <v>15</v>
@@ -5219,7 +5234,7 @@
         <v>3</v>
       </c>
       <c r="N41" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O41" s="16" t="s">
         <v>17</v>
@@ -5231,19 +5246,19 @@
         <v>2000</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S41" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T41" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U41" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V41" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>124</v>
@@ -5254,25 +5269,25 @@
         <v>98</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I42" s="15" t="s">
         <v>126</v>
@@ -5290,7 +5305,7 @@
         <v>3</v>
       </c>
       <c r="N42" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O42" s="15" t="s">
         <v>17</v>
@@ -5302,22 +5317,22 @@
         <v>2000</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S42" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="T42" s="8">
         <v>2014</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="V42" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>320</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>